<commit_message>
move the driver to project
</commit_message>
<xml_diff>
--- a/TestData/FCCB_TBCL_data.xlsx
+++ b/TestData/FCCB_TBCL_data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu-b\git\PageObjectModel\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF27F3B-FCA1-484C-BCCC-4356EB03ECDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19874A67-0078-4A08-9B98-060B7EDD7D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
   <si>
     <t>fbbs</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -515,40 +515,72 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>06201890101202000000000148</t>
-  </si>
-  <si>
-    <t>06201890101202000000000149</t>
-  </si>
-  <si>
-    <t>C:\Users\liu-b\git\PageObjectModel\screenshot\FCCB_TB_JCX_2_异常截屏_20200630032013588.png</t>
-  </si>
-  <si>
-    <t>未知异常No frame element found by name or id RiskFrame
+    <t>tbr_sj</t>
+  </si>
+  <si>
+    <t>未知弹窗_投保人 李宇轩 的社会统一信用代码错误，请修改！</t>
+  </si>
+  <si>
+    <t>C:\Users\liu-b\git\PageObjectModel\screenshots\FCCB_TB_JCX_1_异常截屏_20200701091358884.png</t>
+  </si>
+  <si>
+    <t>未知异常No frame element found by name or id mainFrame
 Build info: version: '3.14.0', revision: 'aacccce0', time: '2018-08-02T20:19:58.91Z'
-System info: host: 'DESKTOP-I9S3ABE', ip: '100.100.94.239', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_101'
+System info: host: 'DESKTOP-I9S3ABE', ip: '100.100.92.227', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_101'
 Driver info: driver.version: unknown</t>
   </si>
   <si>
-    <t>未知异常Currently focused window has been closed.
+    <t>06201890101202000000000159</t>
+  </si>
+  <si>
+    <t>C:\Users\liu-b\git\PageObjectModel\screenshots\FCCB_TB_JCX_2_未知弹窗_20200701110022974.png</t>
+  </si>
+  <si>
+    <t>06201890101202000000000158</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>06201890101202000000000160</t>
+  </si>
+  <si>
+    <t>C:\Users\liu-b\git\PageObjectModel\screenshots\FCCB_TB_JCX_2_未知弹窗_20200701021926699.png</t>
+  </si>
+  <si>
+    <t>06201890101202000000000169</t>
+  </si>
+  <si>
+    <t>06201890101202000000000170</t>
+  </si>
+  <si>
+    <t>C:\Users\liu-b\git\PageObjectModel\screenshots\FCCB_TB_JCX_2_未知弹窗_20200701044658634.png</t>
+  </si>
+  <si>
+    <t>C:\Users\liu-b\git\PageObjectModel\screenshots\FCCB_TB_JCX_1_异常截屏_20200701060502602.png</t>
+  </si>
+  <si>
+    <t>未知异常No frame element found by name or id mainFrame
 Build info: version: '3.14.0', revision: 'aacccce0', time: '2018-08-02T20:19:58.91Z'
-System info: host: 'DESKTOP-I9S3ABE', ip: '100.100.94.239', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_101'
-Driver info: org.openqa.selenium.ie.InternetExplorerDriver
-Capabilities {acceptInsecureCerts: false, browserName: internet explorer, browserVersion: 11, javascriptEnabled: true, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), se:ieOptions: {browserAttachTimeout: 0, elementScrollBehavior: 0, enablePersistentHover: true, ie.browserCommandLineSwitches: , ie.ensureCleanSession: false, ie.fileUploadDialogTimeout: 3000, ie.forceCreateProcessApi: false, ignoreProtectedModeSettings: true, ignoreZoomSetting: false, initialBrowserUrl: http://localhost:27086/, nativeEvents: true, requireWindowFocus: false}, setWindowRect: true, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: ignore}
-Session ID: bd9f92f1-016b-4f7d-8f4a-0a3cf60ff988
-*** Element info: {Using=name, value=SelectIt}</t>
-  </si>
-  <si>
-    <t>tbr_sj</t>
+System info: host: 'DESKTOP-I9S3ABE', ip: '100.100.90.19', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_101'
+Driver info: driver.version: unknown</t>
+  </si>
+  <si>
+    <t>C:\Users\liu-b\git\PageObjectModel\screenshots\FCCB_TB_JCX_2_异常截屏_20200701060527927.png</t>
+  </si>
+  <si>
+    <t>06201890101202000000000171</t>
+  </si>
+  <si>
+    <t>06201890101202000000000172</t>
+  </si>
+  <si>
+    <t>C:\Users\liu-b\git\PageObjectModel\screenshots\FCCB_TB_JCX_2_未知弹窗_20200701062530719.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <sz val="12"/>
@@ -982,41 +1014,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FB4AF2-2C99-459C-9147-AD7590C3225D}">
   <dimension ref="A1:CA5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="19.125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.125" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.25" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.25" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="12" width="14.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.25" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="16" width="8.75" style="1" collapsed="1"/>
-    <col min="17" max="17" width="20.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="19" width="19.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.75" style="1" collapsed="1"/>
-    <col min="21" max="21" width="12.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="24" width="8.75" style="1" collapsed="1"/>
-    <col min="25" max="25" width="16.625" style="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="39" width="8.75" style="1" collapsed="1"/>
-    <col min="40" max="40" width="8.75" style="1"/>
-    <col min="41" max="47" width="8.75" style="1" collapsed="1"/>
-    <col min="48" max="48" width="15.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="66" width="8.75" style="1" collapsed="1"/>
-    <col min="67" max="67" width="26.75" style="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="76" width="8.75" style="1" collapsed="1"/>
-    <col min="77" max="77" width="17.125" style="1" customWidth="1" collapsed="1"/>
-    <col min="78" max="78" width="16.5" style="1" customWidth="1" collapsed="1"/>
-    <col min="79" max="79" width="25" style="1" customWidth="1" collapsed="1"/>
-    <col min="80" max="16384" width="8.75" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="19.125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="18.75" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="33.125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="9.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="12.25" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="16.375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="8.25" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="11.625" collapsed="true"/>
+    <col min="10" max="12" customWidth="true" style="1" width="14.75" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="18.25" collapsed="true"/>
+    <col min="14" max="16" style="1" width="8.75" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="20.5" collapsed="true"/>
+    <col min="18" max="19" customWidth="true" style="1" width="19.5" collapsed="true"/>
+    <col min="20" max="20" style="1" width="8.75" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="1" width="12.625" collapsed="true"/>
+    <col min="22" max="24" style="1" width="8.75" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="1" width="16.625" collapsed="true"/>
+    <col min="26" max="47" style="1" width="8.75" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" style="1" width="15.5" collapsed="true"/>
+    <col min="49" max="66" style="1" width="8.75" collapsed="true"/>
+    <col min="67" max="67" customWidth="true" style="1" width="26.75" collapsed="true"/>
+    <col min="68" max="76" style="1" width="8.75" collapsed="true"/>
+    <col min="77" max="77" customWidth="true" style="1" width="17.125" collapsed="true"/>
+    <col min="78" max="78" customWidth="true" style="1" width="16.5" collapsed="true"/>
+    <col min="79" max="79" customWidth="true" style="1" width="25.0" collapsed="true"/>
+    <col min="80" max="16384" style="1" width="8.75" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:79">
@@ -1237,7 +1267,7 @@
         <v>46</v>
       </c>
       <c r="AN2" s="6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="AO2" s="6" t="s">
         <v>47</v>
@@ -1525,13 +1555,13 @@
         <v>107</v>
       </c>
       <c r="BY3" s="4" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="BZ3" s="4" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="CA3" s="4" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:79">
@@ -1702,13 +1732,13 @@
         <v>107</v>
       </c>
       <c r="BY4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="BZ4" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="BZ4" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="CA4" s="4" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:79">

</xml_diff>